<commit_message>
ADD tablas tags y platforms
</commit_message>
<xml_diff>
--- a/uploads/products.xlsx
+++ b/uploads/products.xlsx
@@ -46,7 +46,7 @@
     <t xml:space="preserve">is_offer</t>
   </si>
   <si>
-    <t xml:space="preserve">offer_value</t>
+    <t xml:space="preserve">offer_percentage</t>
   </si>
   <si>
     <t xml:space="preserve">offer_start_date</t>
@@ -115,7 +115,7 @@
     <t xml:space="preserve">La saga looter-shooter regresa con más acción, humor y caos que nunca. Borderlands 4 ofrece intensos combates en primera persona, millones de armas, habilidades únicas y un estilo visual inconfundible. Juega en solitario o en cooperativo y enfréntate a enemigos desbordantes de personalidad en un universo lleno de locura y diversión.</t>
   </si>
   <si>
-    <t xml:space="preserve">cover_borderlands4</t>
+    <t xml:space="preserve">cover_borderlands4.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">P00005</t>
@@ -157,13 +157,13 @@
     <t xml:space="preserve">P00008</t>
   </si>
   <si>
-    <t xml:space="preserve">Pokemon Leyends Z/A</t>
+    <t xml:space="preserve">Pokemon Legends Z/A</t>
   </si>
   <si>
     <t xml:space="preserve">Explora una nueva visión del mundo Pokémon con Pokémon Legends: Z-A. Este título apuesta por una jugabilidad renovada, exploración más libre y una narrativa diferente a la saga principal. Descubre nuevas mecánicas, Pokémon y una historia ambientada en una región icónica reinventada.</t>
   </si>
   <si>
-    <t xml:space="preserve">cover_pokemon_leyends_ZA.jpg</t>
+    <t xml:space="preserve">cover_pokemon_legends_ZA.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">P00009</t>
@@ -411,8 +411,8 @@
   </sheetPr>
   <dimension ref="A1:M20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I16" activeCellId="0" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -423,7 +423,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="15.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="8.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="7.97"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="11.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="15.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="14.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="14.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="12.28"/>

</xml_diff>

<commit_message>
ADD Estructura funcional de header, footer, productos, producto y estilos
</commit_message>
<xml_diff>
--- a/uploads/products.xlsx
+++ b/uploads/products.xlsx
@@ -266,7 +266,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -411,13 +411,13 @@
   </sheetPr>
   <dimension ref="A1:M20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I16" activeCellId="0" sqref="I16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="24.93"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="27.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="15.9"/>
@@ -472,7 +472,7 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -501,7 +501,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B3" s="5" t="s">
@@ -530,7 +530,7 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -559,7 +559,7 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -588,7 +588,7 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -617,7 +617,7 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -646,7 +646,7 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -675,7 +675,7 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -704,7 +704,7 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="1" t="s">
         <v>48</v>
       </c>
       <c r="B10" s="1" t="s">

</xml_diff>